<commit_message>
feat: add excel pie chart and write-up
</commit_message>
<xml_diff>
--- a/02_activities/assignments/assignment_3/Marriage Licence Statistics Data.xlsx
+++ b/02_activities/assignments/assignment_3/Marriage Licence Statistics Data.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pca_9\Desktop\visualization\02_activities\assignments\assignment_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C19DAF0-0C19-4D28-B95C-016E9F3602CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E6D1D1DB-A223-453C-9D05-FE24F365035E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="4236"/>
   </bookViews>
   <sheets>
-    <sheet name="Marriage Licence Statistics Dat" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Marriage Licence Statistics Dat" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="9" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="192">
   <si>
     <t>_id</t>
   </si>
@@ -587,6 +591,15 @@
   </si>
   <si>
     <t>2026-01</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of MARRIAGE_LICENSES</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1083,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1128,6 +1146,4734 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Marriage Licence Statistics Data.xlsx]Sheet2!PivotTable4</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:pattFill prst="pct75">
+              <a:fgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:sysClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:sysClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>ET</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NY</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>19624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D52-43DC-BB2E-A4EA2461B37A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FBBC507-6181-457C-A0F3-997C9ED0BE41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="CHIANG AIK Pun" refreshedDate="46056.001191319447" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="578">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D579" sheet="Marriage Licence Statistics Dat"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="_id" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="24901" maxValue="25478"/>
+    </cacheField>
+    <cacheField name="CIVIC_CENTRE" numFmtId="0">
+      <sharedItems count="4">
+        <s v="ET"/>
+        <s v="NY"/>
+        <s v="SC"/>
+        <s v="TO"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="MARRIAGE_LICENSES" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1773"/>
+    </cacheField>
+    <cacheField name="TIME_PERIOD" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="578">
+  <r>
+    <n v="24901"/>
+    <x v="0"/>
+    <n v="80"/>
+    <s v="2011-01"/>
+  </r>
+  <r>
+    <n v="24902"/>
+    <x v="1"/>
+    <n v="136"/>
+    <s v="2011-01"/>
+  </r>
+  <r>
+    <n v="24903"/>
+    <x v="2"/>
+    <n v="159"/>
+    <s v="2011-01"/>
+  </r>
+  <r>
+    <n v="24904"/>
+    <x v="3"/>
+    <n v="367"/>
+    <s v="2011-01"/>
+  </r>
+  <r>
+    <n v="24905"/>
+    <x v="0"/>
+    <n v="109"/>
+    <s v="2011-02"/>
+  </r>
+  <r>
+    <n v="24906"/>
+    <x v="1"/>
+    <n v="150"/>
+    <s v="2011-02"/>
+  </r>
+  <r>
+    <n v="24907"/>
+    <x v="2"/>
+    <n v="154"/>
+    <s v="2011-02"/>
+  </r>
+  <r>
+    <n v="24908"/>
+    <x v="3"/>
+    <n v="383"/>
+    <s v="2011-02"/>
+  </r>
+  <r>
+    <n v="24909"/>
+    <x v="0"/>
+    <n v="177"/>
+    <s v="2011-03"/>
+  </r>
+  <r>
+    <n v="24910"/>
+    <x v="1"/>
+    <n v="231"/>
+    <s v="2011-03"/>
+  </r>
+  <r>
+    <n v="24911"/>
+    <x v="2"/>
+    <n v="213"/>
+    <s v="2011-03"/>
+  </r>
+  <r>
+    <n v="24912"/>
+    <x v="3"/>
+    <n v="589"/>
+    <s v="2011-03"/>
+  </r>
+  <r>
+    <n v="24913"/>
+    <x v="0"/>
+    <n v="178"/>
+    <s v="2011-04"/>
+  </r>
+  <r>
+    <n v="24914"/>
+    <x v="1"/>
+    <n v="277"/>
+    <s v="2011-04"/>
+  </r>
+  <r>
+    <n v="24915"/>
+    <x v="2"/>
+    <n v="261"/>
+    <s v="2011-04"/>
+  </r>
+  <r>
+    <n v="24916"/>
+    <x v="3"/>
+    <n v="660"/>
+    <s v="2011-04"/>
+  </r>
+  <r>
+    <n v="24917"/>
+    <x v="0"/>
+    <n v="263"/>
+    <s v="2011-05"/>
+  </r>
+  <r>
+    <n v="24918"/>
+    <x v="1"/>
+    <n v="376"/>
+    <s v="2011-05"/>
+  </r>
+  <r>
+    <n v="24919"/>
+    <x v="2"/>
+    <n v="375"/>
+    <s v="2011-05"/>
+  </r>
+  <r>
+    <n v="24920"/>
+    <x v="3"/>
+    <n v="871"/>
+    <s v="2011-05"/>
+  </r>
+  <r>
+    <n v="24921"/>
+    <x v="0"/>
+    <n v="255"/>
+    <s v="2011-06"/>
+  </r>
+  <r>
+    <n v="24922"/>
+    <x v="1"/>
+    <n v="365"/>
+    <s v="2011-06"/>
+  </r>
+  <r>
+    <n v="24923"/>
+    <x v="2"/>
+    <n v="334"/>
+    <s v="2011-06"/>
+  </r>
+  <r>
+    <n v="24924"/>
+    <x v="3"/>
+    <n v="870"/>
+    <s v="2011-06"/>
+  </r>
+  <r>
+    <n v="24925"/>
+    <x v="0"/>
+    <n v="238"/>
+    <s v="2011-07"/>
+  </r>
+  <r>
+    <n v="24926"/>
+    <x v="1"/>
+    <n v="364"/>
+    <s v="2011-07"/>
+  </r>
+  <r>
+    <n v="24927"/>
+    <x v="2"/>
+    <n v="352"/>
+    <s v="2011-07"/>
+  </r>
+  <r>
+    <n v="24928"/>
+    <x v="3"/>
+    <n v="989"/>
+    <s v="2011-07"/>
+  </r>
+  <r>
+    <n v="24929"/>
+    <x v="0"/>
+    <n v="257"/>
+    <s v="2011-08"/>
+  </r>
+  <r>
+    <n v="24930"/>
+    <x v="1"/>
+    <n v="366"/>
+    <s v="2011-08"/>
+  </r>
+  <r>
+    <n v="24931"/>
+    <x v="2"/>
+    <n v="345"/>
+    <s v="2011-08"/>
+  </r>
+  <r>
+    <n v="24932"/>
+    <x v="3"/>
+    <n v="965"/>
+    <s v="2011-08"/>
+  </r>
+  <r>
+    <n v="24933"/>
+    <x v="0"/>
+    <n v="152"/>
+    <s v="2011-09"/>
+  </r>
+  <r>
+    <n v="24934"/>
+    <x v="1"/>
+    <n v="255"/>
+    <s v="2011-09"/>
+  </r>
+  <r>
+    <n v="24935"/>
+    <x v="2"/>
+    <n v="276"/>
+    <s v="2011-09"/>
+  </r>
+  <r>
+    <n v="24936"/>
+    <x v="3"/>
+    <n v="638"/>
+    <s v="2011-09"/>
+  </r>
+  <r>
+    <n v="24937"/>
+    <x v="0"/>
+    <n v="126"/>
+    <s v="2011-10"/>
+  </r>
+  <r>
+    <n v="24938"/>
+    <x v="1"/>
+    <n v="201"/>
+    <s v="2011-10"/>
+  </r>
+  <r>
+    <n v="24939"/>
+    <x v="2"/>
+    <n v="218"/>
+    <s v="2011-10"/>
+  </r>
+  <r>
+    <n v="24940"/>
+    <x v="3"/>
+    <n v="468"/>
+    <s v="2011-10"/>
+  </r>
+  <r>
+    <n v="24941"/>
+    <x v="0"/>
+    <n v="103"/>
+    <s v="2011-11"/>
+  </r>
+  <r>
+    <n v="24942"/>
+    <x v="1"/>
+    <n v="191"/>
+    <s v="2011-11"/>
+  </r>
+  <r>
+    <n v="24943"/>
+    <x v="2"/>
+    <n v="182"/>
+    <s v="2011-11"/>
+  </r>
+  <r>
+    <n v="24944"/>
+    <x v="3"/>
+    <n v="340"/>
+    <s v="2011-11"/>
+  </r>
+  <r>
+    <n v="24945"/>
+    <x v="0"/>
+    <n v="109"/>
+    <s v="2011-12"/>
+  </r>
+  <r>
+    <n v="24946"/>
+    <x v="1"/>
+    <n v="171"/>
+    <s v="2011-12"/>
+  </r>
+  <r>
+    <n v="24947"/>
+    <x v="2"/>
+    <n v="149"/>
+    <s v="2011-12"/>
+  </r>
+  <r>
+    <n v="24948"/>
+    <x v="3"/>
+    <n v="356"/>
+    <s v="2011-12"/>
+  </r>
+  <r>
+    <n v="24949"/>
+    <x v="0"/>
+    <n v="115"/>
+    <s v="2012-01"/>
+  </r>
+  <r>
+    <n v="24950"/>
+    <x v="1"/>
+    <n v="176"/>
+    <s v="2012-01"/>
+  </r>
+  <r>
+    <n v="24951"/>
+    <x v="2"/>
+    <n v="171"/>
+    <s v="2012-01"/>
+  </r>
+  <r>
+    <n v="24952"/>
+    <x v="3"/>
+    <n v="440"/>
+    <s v="2012-01"/>
+  </r>
+  <r>
+    <n v="24953"/>
+    <x v="0"/>
+    <n v="134"/>
+    <s v="2012-02"/>
+  </r>
+  <r>
+    <n v="24954"/>
+    <x v="1"/>
+    <n v="195"/>
+    <s v="2012-02"/>
+  </r>
+  <r>
+    <n v="24955"/>
+    <x v="2"/>
+    <n v="160"/>
+    <s v="2012-02"/>
+  </r>
+  <r>
+    <n v="24956"/>
+    <x v="3"/>
+    <n v="390"/>
+    <s v="2012-02"/>
+  </r>
+  <r>
+    <n v="24957"/>
+    <x v="0"/>
+    <n v="183"/>
+    <s v="2012-03"/>
+  </r>
+  <r>
+    <n v="24958"/>
+    <x v="1"/>
+    <n v="234"/>
+    <s v="2012-03"/>
+  </r>
+  <r>
+    <n v="24959"/>
+    <x v="2"/>
+    <n v="243"/>
+    <s v="2012-03"/>
+  </r>
+  <r>
+    <n v="24960"/>
+    <x v="3"/>
+    <n v="567"/>
+    <s v="2012-03"/>
+  </r>
+  <r>
+    <n v="24961"/>
+    <x v="0"/>
+    <n v="194"/>
+    <s v="2012-04"/>
+  </r>
+  <r>
+    <n v="24962"/>
+    <x v="1"/>
+    <n v="225"/>
+    <s v="2012-04"/>
+  </r>
+  <r>
+    <n v="24963"/>
+    <x v="2"/>
+    <n v="252"/>
+    <s v="2012-04"/>
+  </r>
+  <r>
+    <n v="24964"/>
+    <x v="3"/>
+    <n v="561"/>
+    <s v="2012-04"/>
+  </r>
+  <r>
+    <n v="24965"/>
+    <x v="0"/>
+    <n v="217"/>
+    <s v="2012-05"/>
+  </r>
+  <r>
+    <n v="24966"/>
+    <x v="1"/>
+    <n v="294"/>
+    <s v="2012-05"/>
+  </r>
+  <r>
+    <n v="24967"/>
+    <x v="2"/>
+    <n v="332"/>
+    <s v="2012-05"/>
+  </r>
+  <r>
+    <n v="24968"/>
+    <x v="3"/>
+    <n v="807"/>
+    <s v="2012-05"/>
+  </r>
+  <r>
+    <n v="24969"/>
+    <x v="0"/>
+    <n v="262"/>
+    <s v="2012-06"/>
+  </r>
+  <r>
+    <n v="24970"/>
+    <x v="1"/>
+    <n v="353"/>
+    <s v="2012-06"/>
+  </r>
+  <r>
+    <n v="24971"/>
+    <x v="2"/>
+    <n v="340"/>
+    <s v="2012-06"/>
+  </r>
+  <r>
+    <n v="24972"/>
+    <x v="3"/>
+    <n v="888"/>
+    <s v="2012-06"/>
+  </r>
+  <r>
+    <n v="24973"/>
+    <x v="0"/>
+    <n v="269"/>
+    <s v="2012-07"/>
+  </r>
+  <r>
+    <n v="24974"/>
+    <x v="1"/>
+    <n v="404"/>
+    <s v="2012-07"/>
+  </r>
+  <r>
+    <n v="24975"/>
+    <x v="2"/>
+    <n v="371"/>
+    <s v="2012-07"/>
+  </r>
+  <r>
+    <n v="24976"/>
+    <x v="3"/>
+    <n v="971"/>
+    <s v="2012-07"/>
+  </r>
+  <r>
+    <n v="24977"/>
+    <x v="0"/>
+    <n v="251"/>
+    <s v="2012-08"/>
+  </r>
+  <r>
+    <n v="24978"/>
+    <x v="1"/>
+    <n v="353"/>
+    <s v="2012-08"/>
+  </r>
+  <r>
+    <n v="24979"/>
+    <x v="2"/>
+    <n v="346"/>
+    <s v="2012-08"/>
+  </r>
+  <r>
+    <n v="24980"/>
+    <x v="3"/>
+    <n v="980"/>
+    <s v="2012-08"/>
+  </r>
+  <r>
+    <n v="24981"/>
+    <x v="0"/>
+    <n v="132"/>
+    <s v="2012-09"/>
+  </r>
+  <r>
+    <n v="24982"/>
+    <x v="1"/>
+    <n v="233"/>
+    <s v="2012-09"/>
+  </r>
+  <r>
+    <n v="24983"/>
+    <x v="2"/>
+    <n v="215"/>
+    <s v="2012-09"/>
+  </r>
+  <r>
+    <n v="24984"/>
+    <x v="3"/>
+    <n v="563"/>
+    <s v="2012-09"/>
+  </r>
+  <r>
+    <n v="24985"/>
+    <x v="0"/>
+    <n v="156"/>
+    <s v="2012-10"/>
+  </r>
+  <r>
+    <n v="24986"/>
+    <x v="1"/>
+    <n v="208"/>
+    <s v="2012-10"/>
+  </r>
+  <r>
+    <n v="24987"/>
+    <x v="2"/>
+    <n v="215"/>
+    <s v="2012-10"/>
+  </r>
+  <r>
+    <n v="24988"/>
+    <x v="3"/>
+    <n v="486"/>
+    <s v="2012-10"/>
+  </r>
+  <r>
+    <n v="24989"/>
+    <x v="0"/>
+    <n v="85"/>
+    <s v="2012-11"/>
+  </r>
+  <r>
+    <n v="24990"/>
+    <x v="1"/>
+    <n v="180"/>
+    <s v="2012-11"/>
+  </r>
+  <r>
+    <n v="24991"/>
+    <x v="2"/>
+    <n v="170"/>
+    <s v="2012-11"/>
+  </r>
+  <r>
+    <n v="24992"/>
+    <x v="3"/>
+    <n v="391"/>
+    <s v="2012-11"/>
+  </r>
+  <r>
+    <n v="24993"/>
+    <x v="0"/>
+    <n v="99"/>
+    <s v="2012-12"/>
+  </r>
+  <r>
+    <n v="24994"/>
+    <x v="1"/>
+    <n v="163"/>
+    <s v="2012-12"/>
+  </r>
+  <r>
+    <n v="24995"/>
+    <x v="2"/>
+    <n v="158"/>
+    <s v="2012-12"/>
+  </r>
+  <r>
+    <n v="24996"/>
+    <x v="3"/>
+    <n v="365"/>
+    <s v="2012-12"/>
+  </r>
+  <r>
+    <n v="24997"/>
+    <x v="0"/>
+    <n v="91"/>
+    <s v="2013-01"/>
+  </r>
+  <r>
+    <n v="24998"/>
+    <x v="1"/>
+    <n v="169"/>
+    <s v="2013-01"/>
+  </r>
+  <r>
+    <n v="24999"/>
+    <x v="2"/>
+    <n v="138"/>
+    <s v="2013-01"/>
+  </r>
+  <r>
+    <n v="25000"/>
+    <x v="3"/>
+    <n v="365"/>
+    <s v="2013-01"/>
+  </r>
+  <r>
+    <n v="25001"/>
+    <x v="0"/>
+    <n v="90"/>
+    <s v="2013-02"/>
+  </r>
+  <r>
+    <n v="25002"/>
+    <x v="1"/>
+    <n v="163"/>
+    <s v="2013-02"/>
+  </r>
+  <r>
+    <n v="25003"/>
+    <x v="2"/>
+    <n v="126"/>
+    <s v="2013-02"/>
+  </r>
+  <r>
+    <n v="25004"/>
+    <x v="3"/>
+    <n v="346"/>
+    <s v="2013-02"/>
+  </r>
+  <r>
+    <n v="25005"/>
+    <x v="0"/>
+    <n v="130"/>
+    <s v="2013-03"/>
+  </r>
+  <r>
+    <n v="25006"/>
+    <x v="1"/>
+    <n v="217"/>
+    <s v="2013-03"/>
+  </r>
+  <r>
+    <n v="25007"/>
+    <x v="2"/>
+    <n v="188"/>
+    <s v="2013-03"/>
+  </r>
+  <r>
+    <n v="25008"/>
+    <x v="3"/>
+    <n v="455"/>
+    <s v="2013-03"/>
+  </r>
+  <r>
+    <n v="25009"/>
+    <x v="0"/>
+    <n v="177"/>
+    <s v="2013-04"/>
+  </r>
+  <r>
+    <n v="25010"/>
+    <x v="1"/>
+    <n v="298"/>
+    <s v="2013-04"/>
+  </r>
+  <r>
+    <n v="25011"/>
+    <x v="2"/>
+    <n v="219"/>
+    <s v="2013-04"/>
+  </r>
+  <r>
+    <n v="25012"/>
+    <x v="3"/>
+    <n v="666"/>
+    <s v="2013-04"/>
+  </r>
+  <r>
+    <n v="25013"/>
+    <x v="0"/>
+    <n v="223"/>
+    <s v="2013-05"/>
+  </r>
+  <r>
+    <n v="25014"/>
+    <x v="1"/>
+    <n v="310"/>
+    <s v="2013-05"/>
+  </r>
+  <r>
+    <n v="25015"/>
+    <x v="2"/>
+    <n v="300"/>
+    <s v="2013-05"/>
+  </r>
+  <r>
+    <n v="25016"/>
+    <x v="3"/>
+    <n v="748"/>
+    <s v="2013-05"/>
+  </r>
+  <r>
+    <n v="25017"/>
+    <x v="0"/>
+    <n v="212"/>
+    <s v="2013-06"/>
+  </r>
+  <r>
+    <n v="25018"/>
+    <x v="1"/>
+    <n v="286"/>
+    <s v="2013-06"/>
+  </r>
+  <r>
+    <n v="25019"/>
+    <x v="2"/>
+    <n v="303"/>
+    <s v="2013-06"/>
+  </r>
+  <r>
+    <n v="25020"/>
+    <x v="3"/>
+    <n v="778"/>
+    <s v="2013-06"/>
+  </r>
+  <r>
+    <n v="25021"/>
+    <x v="0"/>
+    <n v="258"/>
+    <s v="2013-07"/>
+  </r>
+  <r>
+    <n v="25022"/>
+    <x v="1"/>
+    <n v="450"/>
+    <s v="2013-07"/>
+  </r>
+  <r>
+    <n v="25023"/>
+    <x v="2"/>
+    <n v="319"/>
+    <s v="2013-07"/>
+  </r>
+  <r>
+    <n v="25024"/>
+    <x v="3"/>
+    <n v="972"/>
+    <s v="2013-07"/>
+  </r>
+  <r>
+    <n v="25025"/>
+    <x v="0"/>
+    <n v="244"/>
+    <s v="2013-08"/>
+  </r>
+  <r>
+    <n v="25026"/>
+    <x v="1"/>
+    <n v="324"/>
+    <s v="2013-08"/>
+  </r>
+  <r>
+    <n v="25027"/>
+    <x v="2"/>
+    <n v="322"/>
+    <s v="2013-08"/>
+  </r>
+  <r>
+    <n v="25028"/>
+    <x v="3"/>
+    <n v="931"/>
+    <s v="2013-08"/>
+  </r>
+  <r>
+    <n v="25029"/>
+    <x v="0"/>
+    <n v="157"/>
+    <s v="2013-09"/>
+  </r>
+  <r>
+    <n v="25030"/>
+    <x v="1"/>
+    <n v="232"/>
+    <s v="2013-09"/>
+  </r>
+  <r>
+    <n v="25031"/>
+    <x v="2"/>
+    <n v="233"/>
+    <s v="2013-09"/>
+  </r>
+  <r>
+    <n v="25032"/>
+    <x v="3"/>
+    <n v="607"/>
+    <s v="2013-09"/>
+  </r>
+  <r>
+    <n v="25033"/>
+    <x v="0"/>
+    <n v="121"/>
+    <s v="2013-10"/>
+  </r>
+  <r>
+    <n v="25034"/>
+    <x v="1"/>
+    <n v="163"/>
+    <s v="2013-10"/>
+  </r>
+  <r>
+    <n v="25035"/>
+    <x v="2"/>
+    <n v="208"/>
+    <s v="2013-10"/>
+  </r>
+  <r>
+    <n v="25036"/>
+    <x v="3"/>
+    <n v="448"/>
+    <s v="2013-10"/>
+  </r>
+  <r>
+    <n v="25037"/>
+    <x v="0"/>
+    <n v="92"/>
+    <s v="2013-11"/>
+  </r>
+  <r>
+    <n v="25038"/>
+    <x v="1"/>
+    <n v="162"/>
+    <s v="2013-11"/>
+  </r>
+  <r>
+    <n v="25039"/>
+    <x v="2"/>
+    <n v="140"/>
+    <s v="2013-11"/>
+  </r>
+  <r>
+    <n v="25040"/>
+    <x v="3"/>
+    <n v="315"/>
+    <s v="2013-11"/>
+  </r>
+  <r>
+    <n v="25041"/>
+    <x v="0"/>
+    <n v="89"/>
+    <s v="2013-12"/>
+  </r>
+  <r>
+    <n v="25042"/>
+    <x v="1"/>
+    <n v="146"/>
+    <s v="2013-12"/>
+  </r>
+  <r>
+    <n v="25043"/>
+    <x v="2"/>
+    <n v="130"/>
+    <s v="2013-12"/>
+  </r>
+  <r>
+    <n v="25044"/>
+    <x v="3"/>
+    <n v="314"/>
+    <s v="2013-12"/>
+  </r>
+  <r>
+    <n v="25045"/>
+    <x v="0"/>
+    <n v="85"/>
+    <s v="2014-01"/>
+  </r>
+  <r>
+    <n v="25046"/>
+    <x v="1"/>
+    <n v="186"/>
+    <s v="2014-01"/>
+  </r>
+  <r>
+    <n v="25047"/>
+    <x v="2"/>
+    <n v="139"/>
+    <s v="2014-01"/>
+  </r>
+  <r>
+    <n v="25048"/>
+    <x v="3"/>
+    <n v="375"/>
+    <s v="2014-01"/>
+  </r>
+  <r>
+    <n v="25049"/>
+    <x v="0"/>
+    <n v="93"/>
+    <s v="2014-02"/>
+  </r>
+  <r>
+    <n v="25050"/>
+    <x v="1"/>
+    <n v="134"/>
+    <s v="2014-02"/>
+  </r>
+  <r>
+    <n v="25051"/>
+    <x v="2"/>
+    <n v="126"/>
+    <s v="2014-02"/>
+  </r>
+  <r>
+    <n v="25052"/>
+    <x v="3"/>
+    <n v="364"/>
+    <s v="2014-02"/>
+  </r>
+  <r>
+    <n v="25053"/>
+    <x v="0"/>
+    <n v="151"/>
+    <s v="2014-03"/>
+  </r>
+  <r>
+    <n v="25054"/>
+    <x v="1"/>
+    <n v="201"/>
+    <s v="2014-03"/>
+  </r>
+  <r>
+    <n v="25055"/>
+    <x v="2"/>
+    <n v="180"/>
+    <s v="2014-03"/>
+  </r>
+  <r>
+    <n v="25056"/>
+    <x v="3"/>
+    <n v="530"/>
+    <s v="2014-03"/>
+  </r>
+  <r>
+    <n v="25057"/>
+    <x v="0"/>
+    <n v="151"/>
+    <s v="2014-04"/>
+  </r>
+  <r>
+    <n v="25058"/>
+    <x v="1"/>
+    <n v="240"/>
+    <s v="2014-04"/>
+  </r>
+  <r>
+    <n v="25059"/>
+    <x v="2"/>
+    <n v="229"/>
+    <s v="2014-04"/>
+  </r>
+  <r>
+    <n v="25060"/>
+    <x v="3"/>
+    <n v="674"/>
+    <s v="2014-04"/>
+  </r>
+  <r>
+    <n v="25061"/>
+    <x v="0"/>
+    <n v="219"/>
+    <s v="2014-05"/>
+  </r>
+  <r>
+    <n v="25062"/>
+    <x v="1"/>
+    <n v="318"/>
+    <s v="2014-05"/>
+  </r>
+  <r>
+    <n v="25063"/>
+    <x v="2"/>
+    <n v="298"/>
+    <s v="2014-05"/>
+  </r>
+  <r>
+    <n v="25064"/>
+    <x v="3"/>
+    <n v="847"/>
+    <s v="2014-05"/>
+  </r>
+  <r>
+    <n v="25065"/>
+    <x v="0"/>
+    <n v="240"/>
+    <s v="2014-06"/>
+  </r>
+  <r>
+    <n v="25066"/>
+    <x v="1"/>
+    <n v="309"/>
+    <s v="2014-06"/>
+  </r>
+  <r>
+    <n v="25067"/>
+    <x v="2"/>
+    <n v="315"/>
+    <s v="2014-06"/>
+  </r>
+  <r>
+    <n v="25068"/>
+    <x v="3"/>
+    <n v="942"/>
+    <s v="2014-06"/>
+  </r>
+  <r>
+    <n v="25069"/>
+    <x v="0"/>
+    <n v="252"/>
+    <s v="2014-07"/>
+  </r>
+  <r>
+    <n v="25070"/>
+    <x v="1"/>
+    <n v="348"/>
+    <s v="2014-07"/>
+  </r>
+  <r>
+    <n v="25071"/>
+    <x v="2"/>
+    <n v="338"/>
+    <s v="2014-07"/>
+  </r>
+  <r>
+    <n v="25072"/>
+    <x v="3"/>
+    <n v="1024"/>
+    <s v="2014-07"/>
+  </r>
+  <r>
+    <n v="25073"/>
+    <x v="0"/>
+    <n v="239"/>
+    <s v="2014-08"/>
+  </r>
+  <r>
+    <n v="25074"/>
+    <x v="1"/>
+    <n v="351"/>
+    <s v="2014-08"/>
+  </r>
+  <r>
+    <n v="25075"/>
+    <x v="2"/>
+    <n v="288"/>
+    <s v="2014-08"/>
+  </r>
+  <r>
+    <n v="25076"/>
+    <x v="3"/>
+    <n v="967"/>
+    <s v="2014-08"/>
+  </r>
+  <r>
+    <n v="25077"/>
+    <x v="0"/>
+    <n v="169"/>
+    <s v="2014-09"/>
+  </r>
+  <r>
+    <n v="25078"/>
+    <x v="1"/>
+    <n v="228"/>
+    <s v="2014-09"/>
+  </r>
+  <r>
+    <n v="25079"/>
+    <x v="2"/>
+    <n v="225"/>
+    <s v="2014-09"/>
+  </r>
+  <r>
+    <n v="25080"/>
+    <x v="3"/>
+    <n v="658"/>
+    <s v="2014-09"/>
+  </r>
+  <r>
+    <n v="25081"/>
+    <x v="0"/>
+    <n v="126"/>
+    <s v="2014-10"/>
+  </r>
+  <r>
+    <n v="25082"/>
+    <x v="1"/>
+    <n v="180"/>
+    <s v="2014-10"/>
+  </r>
+  <r>
+    <n v="25083"/>
+    <x v="2"/>
+    <n v="206"/>
+    <s v="2014-10"/>
+  </r>
+  <r>
+    <n v="25084"/>
+    <x v="3"/>
+    <n v="489"/>
+    <s v="2014-10"/>
+  </r>
+  <r>
+    <n v="25085"/>
+    <x v="0"/>
+    <n v="77"/>
+    <s v="2014-11"/>
+  </r>
+  <r>
+    <n v="25086"/>
+    <x v="1"/>
+    <n v="138"/>
+    <s v="2014-11"/>
+  </r>
+  <r>
+    <n v="25087"/>
+    <x v="2"/>
+    <n v="111"/>
+    <s v="2014-11"/>
+  </r>
+  <r>
+    <n v="25088"/>
+    <x v="3"/>
+    <n v="347"/>
+    <s v="2014-11"/>
+  </r>
+  <r>
+    <n v="25089"/>
+    <x v="0"/>
+    <n v="109"/>
+    <s v="2014-12"/>
+  </r>
+  <r>
+    <n v="25090"/>
+    <x v="1"/>
+    <n v="162"/>
+    <s v="2014-12"/>
+  </r>
+  <r>
+    <n v="25091"/>
+    <x v="2"/>
+    <n v="157"/>
+    <s v="2014-12"/>
+  </r>
+  <r>
+    <n v="25092"/>
+    <x v="3"/>
+    <n v="357"/>
+    <s v="2014-12"/>
+  </r>
+  <r>
+    <n v="25093"/>
+    <x v="0"/>
+    <n v="123"/>
+    <s v="2015-01"/>
+  </r>
+  <r>
+    <n v="25094"/>
+    <x v="1"/>
+    <n v="140"/>
+    <s v="2015-01"/>
+  </r>
+  <r>
+    <n v="25095"/>
+    <x v="2"/>
+    <n v="149"/>
+    <s v="2015-01"/>
+  </r>
+  <r>
+    <n v="25096"/>
+    <x v="3"/>
+    <n v="327"/>
+    <s v="2015-01"/>
+  </r>
+  <r>
+    <n v="25097"/>
+    <x v="0"/>
+    <n v="108"/>
+    <s v="2015-02"/>
+  </r>
+  <r>
+    <n v="25098"/>
+    <x v="1"/>
+    <n v="159"/>
+    <s v="2015-02"/>
+  </r>
+  <r>
+    <n v="25099"/>
+    <x v="2"/>
+    <n v="130"/>
+    <s v="2015-02"/>
+  </r>
+  <r>
+    <n v="25100"/>
+    <x v="3"/>
+    <n v="333"/>
+    <s v="2015-02"/>
+  </r>
+  <r>
+    <n v="25101"/>
+    <x v="0"/>
+    <n v="155"/>
+    <s v="2015-03"/>
+  </r>
+  <r>
+    <n v="25102"/>
+    <x v="1"/>
+    <n v="224"/>
+    <s v="2015-03"/>
+  </r>
+  <r>
+    <n v="25103"/>
+    <x v="2"/>
+    <n v="222"/>
+    <s v="2015-03"/>
+  </r>
+  <r>
+    <n v="25104"/>
+    <x v="3"/>
+    <n v="559"/>
+    <s v="2015-03"/>
+  </r>
+  <r>
+    <n v="25105"/>
+    <x v="0"/>
+    <n v="149"/>
+    <s v="2015-04"/>
+  </r>
+  <r>
+    <n v="25106"/>
+    <x v="1"/>
+    <n v="273"/>
+    <s v="2015-04"/>
+  </r>
+  <r>
+    <n v="25107"/>
+    <x v="2"/>
+    <n v="257"/>
+    <s v="2015-04"/>
+  </r>
+  <r>
+    <n v="25108"/>
+    <x v="3"/>
+    <n v="665"/>
+    <s v="2015-04"/>
+  </r>
+  <r>
+    <n v="25109"/>
+    <x v="0"/>
+    <n v="245"/>
+    <s v="2015-05"/>
+  </r>
+  <r>
+    <n v="25110"/>
+    <x v="1"/>
+    <n v="307"/>
+    <s v="2015-05"/>
+  </r>
+  <r>
+    <n v="25111"/>
+    <x v="2"/>
+    <n v="306"/>
+    <s v="2015-05"/>
+  </r>
+  <r>
+    <n v="25112"/>
+    <x v="3"/>
+    <n v="805"/>
+    <s v="2015-05"/>
+  </r>
+  <r>
+    <n v="25113"/>
+    <x v="0"/>
+    <n v="268"/>
+    <s v="2015-06"/>
+  </r>
+  <r>
+    <n v="25114"/>
+    <x v="1"/>
+    <n v="386"/>
+    <s v="2015-06"/>
+  </r>
+  <r>
+    <n v="25115"/>
+    <x v="2"/>
+    <n v="346"/>
+    <s v="2015-06"/>
+  </r>
+  <r>
+    <n v="25116"/>
+    <x v="3"/>
+    <n v="927"/>
+    <s v="2015-06"/>
+  </r>
+  <r>
+    <n v="25117"/>
+    <x v="0"/>
+    <n v="317"/>
+    <s v="2015-07"/>
+  </r>
+  <r>
+    <n v="25118"/>
+    <x v="1"/>
+    <n v="387"/>
+    <s v="2015-07"/>
+  </r>
+  <r>
+    <n v="25119"/>
+    <x v="2"/>
+    <n v="390"/>
+    <s v="2015-07"/>
+  </r>
+  <r>
+    <n v="25120"/>
+    <x v="3"/>
+    <n v="1090"/>
+    <s v="2015-07"/>
+  </r>
+  <r>
+    <n v="25121"/>
+    <x v="0"/>
+    <n v="264"/>
+    <s v="2015-08"/>
+  </r>
+  <r>
+    <n v="25122"/>
+    <x v="1"/>
+    <n v="336"/>
+    <s v="2015-08"/>
+  </r>
+  <r>
+    <n v="25123"/>
+    <x v="2"/>
+    <n v="325"/>
+    <s v="2015-08"/>
+  </r>
+  <r>
+    <n v="25124"/>
+    <x v="3"/>
+    <n v="930"/>
+    <s v="2015-08"/>
+  </r>
+  <r>
+    <n v="25125"/>
+    <x v="0"/>
+    <n v="174"/>
+    <s v="2015-09"/>
+  </r>
+  <r>
+    <n v="25126"/>
+    <x v="1"/>
+    <n v="251"/>
+    <s v="2015-09"/>
+  </r>
+  <r>
+    <n v="25127"/>
+    <x v="2"/>
+    <n v="253"/>
+    <s v="2015-09"/>
+  </r>
+  <r>
+    <n v="25128"/>
+    <x v="3"/>
+    <n v="713"/>
+    <s v="2015-09"/>
+  </r>
+  <r>
+    <n v="25129"/>
+    <x v="0"/>
+    <n v="135"/>
+    <s v="2015-10"/>
+  </r>
+  <r>
+    <n v="25130"/>
+    <x v="1"/>
+    <n v="211"/>
+    <s v="2015-10"/>
+  </r>
+  <r>
+    <n v="25131"/>
+    <x v="2"/>
+    <n v="186"/>
+    <s v="2015-10"/>
+  </r>
+  <r>
+    <n v="25132"/>
+    <x v="3"/>
+    <n v="478"/>
+    <s v="2015-10"/>
+  </r>
+  <r>
+    <n v="25133"/>
+    <x v="0"/>
+    <n v="91"/>
+    <s v="2015-11"/>
+  </r>
+  <r>
+    <n v="25134"/>
+    <x v="1"/>
+    <n v="176"/>
+    <s v="2015-11"/>
+  </r>
+  <r>
+    <n v="25135"/>
+    <x v="2"/>
+    <n v="149"/>
+    <s v="2015-11"/>
+  </r>
+  <r>
+    <n v="25136"/>
+    <x v="3"/>
+    <n v="342"/>
+    <s v="2015-11"/>
+  </r>
+  <r>
+    <n v="25137"/>
+    <x v="0"/>
+    <n v="104"/>
+    <s v="2015-12"/>
+  </r>
+  <r>
+    <n v="25138"/>
+    <x v="1"/>
+    <n v="169"/>
+    <s v="2015-12"/>
+  </r>
+  <r>
+    <n v="25139"/>
+    <x v="2"/>
+    <n v="144"/>
+    <s v="2015-12"/>
+  </r>
+  <r>
+    <n v="25140"/>
+    <x v="3"/>
+    <n v="335"/>
+    <s v="2015-12"/>
+  </r>
+  <r>
+    <n v="25141"/>
+    <x v="0"/>
+    <n v="92"/>
+    <s v="2016-01"/>
+  </r>
+  <r>
+    <n v="25142"/>
+    <x v="1"/>
+    <n v="156"/>
+    <s v="2016-01"/>
+  </r>
+  <r>
+    <n v="25143"/>
+    <x v="2"/>
+    <n v="131"/>
+    <s v="2016-01"/>
+  </r>
+  <r>
+    <n v="25144"/>
+    <x v="3"/>
+    <n v="346"/>
+    <s v="2016-01"/>
+  </r>
+  <r>
+    <n v="25145"/>
+    <x v="0"/>
+    <n v="123"/>
+    <s v="2016-02"/>
+  </r>
+  <r>
+    <n v="25146"/>
+    <x v="1"/>
+    <n v="170"/>
+    <s v="2016-02"/>
+  </r>
+  <r>
+    <n v="25147"/>
+    <x v="2"/>
+    <n v="173"/>
+    <s v="2016-02"/>
+  </r>
+  <r>
+    <n v="25148"/>
+    <x v="3"/>
+    <n v="364"/>
+    <s v="2016-02"/>
+  </r>
+  <r>
+    <n v="25149"/>
+    <x v="0"/>
+    <n v="155"/>
+    <s v="2016-03"/>
+  </r>
+  <r>
+    <n v="25150"/>
+    <x v="1"/>
+    <n v="197"/>
+    <s v="2016-03"/>
+  </r>
+  <r>
+    <n v="25151"/>
+    <x v="2"/>
+    <n v="204"/>
+    <s v="2016-03"/>
+  </r>
+  <r>
+    <n v="25152"/>
+    <x v="3"/>
+    <n v="517"/>
+    <s v="2016-03"/>
+  </r>
+  <r>
+    <n v="25153"/>
+    <x v="0"/>
+    <n v="197"/>
+    <s v="2016-04"/>
+  </r>
+  <r>
+    <n v="25154"/>
+    <x v="1"/>
+    <n v="257"/>
+    <s v="2016-04"/>
+  </r>
+  <r>
+    <n v="25155"/>
+    <x v="2"/>
+    <n v="246"/>
+    <s v="2016-04"/>
+  </r>
+  <r>
+    <n v="25156"/>
+    <x v="3"/>
+    <n v="695"/>
+    <s v="2016-04"/>
+  </r>
+  <r>
+    <n v="25157"/>
+    <x v="0"/>
+    <n v="247"/>
+    <s v="2016-05"/>
+  </r>
+  <r>
+    <n v="25158"/>
+    <x v="1"/>
+    <n v="326"/>
+    <s v="2016-05"/>
+  </r>
+  <r>
+    <n v="25159"/>
+    <x v="2"/>
+    <n v="306"/>
+    <s v="2016-05"/>
+  </r>
+  <r>
+    <n v="25160"/>
+    <x v="3"/>
+    <n v="895"/>
+    <s v="2016-05"/>
+  </r>
+  <r>
+    <n v="25161"/>
+    <x v="0"/>
+    <n v="255"/>
+    <s v="2016-06"/>
+  </r>
+  <r>
+    <n v="25162"/>
+    <x v="1"/>
+    <n v="344"/>
+    <s v="2016-06"/>
+  </r>
+  <r>
+    <n v="25163"/>
+    <x v="2"/>
+    <n v="341"/>
+    <s v="2016-06"/>
+  </r>
+  <r>
+    <n v="25164"/>
+    <x v="3"/>
+    <n v="1071"/>
+    <s v="2016-06"/>
+  </r>
+  <r>
+    <n v="25165"/>
+    <x v="0"/>
+    <n v="274"/>
+    <s v="2016-07"/>
+  </r>
+  <r>
+    <n v="25166"/>
+    <x v="1"/>
+    <n v="384"/>
+    <s v="2016-07"/>
+  </r>
+  <r>
+    <n v="25167"/>
+    <x v="2"/>
+    <n v="348"/>
+    <s v="2016-07"/>
+  </r>
+  <r>
+    <n v="25168"/>
+    <x v="3"/>
+    <n v="1041"/>
+    <s v="2016-07"/>
+  </r>
+  <r>
+    <n v="25169"/>
+    <x v="0"/>
+    <n v="296"/>
+    <s v="2016-08"/>
+  </r>
+  <r>
+    <n v="25170"/>
+    <x v="1"/>
+    <n v="358"/>
+    <s v="2016-08"/>
+  </r>
+  <r>
+    <n v="25171"/>
+    <x v="2"/>
+    <n v="333"/>
+    <s v="2016-08"/>
+  </r>
+  <r>
+    <n v="25172"/>
+    <x v="3"/>
+    <n v="1072"/>
+    <s v="2016-08"/>
+  </r>
+  <r>
+    <n v="25173"/>
+    <x v="0"/>
+    <n v="228"/>
+    <s v="2016-09"/>
+  </r>
+  <r>
+    <n v="25174"/>
+    <x v="1"/>
+    <n v="265"/>
+    <s v="2016-09"/>
+  </r>
+  <r>
+    <n v="25175"/>
+    <x v="2"/>
+    <n v="207"/>
+    <s v="2016-09"/>
+  </r>
+  <r>
+    <n v="25176"/>
+    <x v="3"/>
+    <n v="656"/>
+    <s v="2016-09"/>
+  </r>
+  <r>
+    <n v="25177"/>
+    <x v="0"/>
+    <n v="139"/>
+    <s v="2016-10"/>
+  </r>
+  <r>
+    <n v="25178"/>
+    <x v="1"/>
+    <n v="187"/>
+    <s v="2016-10"/>
+  </r>
+  <r>
+    <n v="25179"/>
+    <x v="2"/>
+    <n v="171"/>
+    <s v="2016-10"/>
+  </r>
+  <r>
+    <n v="25180"/>
+    <x v="3"/>
+    <n v="489"/>
+    <s v="2016-10"/>
+  </r>
+  <r>
+    <n v="25181"/>
+    <x v="0"/>
+    <n v="82"/>
+    <s v="2016-11"/>
+  </r>
+  <r>
+    <n v="25182"/>
+    <x v="1"/>
+    <n v="148"/>
+    <s v="2016-11"/>
+  </r>
+  <r>
+    <n v="25183"/>
+    <x v="2"/>
+    <n v="135"/>
+    <s v="2016-11"/>
+  </r>
+  <r>
+    <n v="25184"/>
+    <x v="3"/>
+    <n v="388"/>
+    <s v="2016-11"/>
+  </r>
+  <r>
+    <n v="25185"/>
+    <x v="0"/>
+    <n v="96"/>
+    <s v="2016-12"/>
+  </r>
+  <r>
+    <n v="25186"/>
+    <x v="1"/>
+    <n v="164"/>
+    <s v="2016-12"/>
+  </r>
+  <r>
+    <n v="25187"/>
+    <x v="2"/>
+    <n v="125"/>
+    <s v="2016-12"/>
+  </r>
+  <r>
+    <n v="25188"/>
+    <x v="3"/>
+    <n v="362"/>
+    <s v="2016-12"/>
+  </r>
+  <r>
+    <n v="25189"/>
+    <x v="0"/>
+    <n v="102"/>
+    <s v="2017-01"/>
+  </r>
+  <r>
+    <n v="25190"/>
+    <x v="1"/>
+    <n v="146"/>
+    <s v="2017-01"/>
+  </r>
+  <r>
+    <n v="25191"/>
+    <x v="2"/>
+    <n v="147"/>
+    <s v="2017-01"/>
+  </r>
+  <r>
+    <n v="25192"/>
+    <x v="3"/>
+    <n v="347"/>
+    <s v="2017-01"/>
+  </r>
+  <r>
+    <n v="25193"/>
+    <x v="0"/>
+    <n v="104"/>
+    <s v="2017-02"/>
+  </r>
+  <r>
+    <n v="25194"/>
+    <x v="1"/>
+    <n v="170"/>
+    <s v="2017-02"/>
+  </r>
+  <r>
+    <n v="25195"/>
+    <x v="2"/>
+    <n v="139"/>
+    <s v="2017-02"/>
+  </r>
+  <r>
+    <n v="25196"/>
+    <x v="3"/>
+    <n v="357"/>
+    <s v="2017-02"/>
+  </r>
+  <r>
+    <n v="25197"/>
+    <x v="0"/>
+    <n v="183"/>
+    <s v="2017-03"/>
+  </r>
+  <r>
+    <n v="25198"/>
+    <x v="1"/>
+    <n v="237"/>
+    <s v="2017-03"/>
+  </r>
+  <r>
+    <n v="25199"/>
+    <x v="2"/>
+    <n v="223"/>
+    <s v="2017-03"/>
+  </r>
+  <r>
+    <n v="25200"/>
+    <x v="3"/>
+    <n v="608"/>
+    <s v="2017-03"/>
+  </r>
+  <r>
+    <n v="25201"/>
+    <x v="0"/>
+    <n v="173"/>
+    <s v="2017-04"/>
+  </r>
+  <r>
+    <n v="25202"/>
+    <x v="1"/>
+    <n v="276"/>
+    <s v="2017-04"/>
+  </r>
+  <r>
+    <n v="25203"/>
+    <x v="2"/>
+    <n v="222"/>
+    <s v="2017-04"/>
+  </r>
+  <r>
+    <n v="25204"/>
+    <x v="3"/>
+    <n v="627"/>
+    <s v="2017-04"/>
+  </r>
+  <r>
+    <n v="25205"/>
+    <x v="0"/>
+    <n v="234"/>
+    <s v="2017-05"/>
+  </r>
+  <r>
+    <n v="25206"/>
+    <x v="1"/>
+    <n v="323"/>
+    <s v="2017-05"/>
+  </r>
+  <r>
+    <n v="25207"/>
+    <x v="2"/>
+    <n v="323"/>
+    <s v="2017-05"/>
+  </r>
+  <r>
+    <n v="25208"/>
+    <x v="3"/>
+    <n v="894"/>
+    <s v="2017-05"/>
+  </r>
+  <r>
+    <n v="25209"/>
+    <x v="0"/>
+    <n v="250"/>
+    <s v="2017-06"/>
+  </r>
+  <r>
+    <n v="25210"/>
+    <x v="1"/>
+    <n v="350"/>
+    <s v="2017-06"/>
+  </r>
+  <r>
+    <n v="25211"/>
+    <x v="2"/>
+    <n v="346"/>
+    <s v="2017-06"/>
+  </r>
+  <r>
+    <n v="25212"/>
+    <x v="3"/>
+    <n v="943"/>
+    <s v="2017-06"/>
+  </r>
+  <r>
+    <n v="25213"/>
+    <x v="0"/>
+    <n v="287"/>
+    <s v="2017-07"/>
+  </r>
+  <r>
+    <n v="25214"/>
+    <x v="1"/>
+    <n v="367"/>
+    <s v="2017-07"/>
+  </r>
+  <r>
+    <n v="25215"/>
+    <x v="2"/>
+    <n v="320"/>
+    <s v="2017-07"/>
+  </r>
+  <r>
+    <n v="25216"/>
+    <x v="3"/>
+    <n v="971"/>
+    <s v="2017-07"/>
+  </r>
+  <r>
+    <n v="25217"/>
+    <x v="0"/>
+    <n v="324"/>
+    <s v="2017-08"/>
+  </r>
+  <r>
+    <n v="25218"/>
+    <x v="1"/>
+    <n v="344"/>
+    <s v="2017-08"/>
+  </r>
+  <r>
+    <n v="25219"/>
+    <x v="2"/>
+    <n v="312"/>
+    <s v="2017-08"/>
+  </r>
+  <r>
+    <n v="25220"/>
+    <x v="3"/>
+    <n v="1066"/>
+    <s v="2017-08"/>
+  </r>
+  <r>
+    <n v="25221"/>
+    <x v="0"/>
+    <n v="207"/>
+    <s v="2017-09"/>
+  </r>
+  <r>
+    <n v="25222"/>
+    <x v="1"/>
+    <n v="268"/>
+    <s v="2017-09"/>
+  </r>
+  <r>
+    <n v="25223"/>
+    <x v="2"/>
+    <n v="233"/>
+    <s v="2017-09"/>
+  </r>
+  <r>
+    <n v="25224"/>
+    <x v="3"/>
+    <n v="729"/>
+    <s v="2017-09"/>
+  </r>
+  <r>
+    <n v="25225"/>
+    <x v="0"/>
+    <n v="144"/>
+    <s v="2017-10"/>
+  </r>
+  <r>
+    <n v="25226"/>
+    <x v="1"/>
+    <n v="219"/>
+    <s v="2017-10"/>
+  </r>
+  <r>
+    <n v="25227"/>
+    <x v="2"/>
+    <n v="194"/>
+    <s v="2017-10"/>
+  </r>
+  <r>
+    <n v="25228"/>
+    <x v="3"/>
+    <n v="552"/>
+    <s v="2017-10"/>
+  </r>
+  <r>
+    <n v="25229"/>
+    <x v="0"/>
+    <n v="98"/>
+    <s v="2017-11"/>
+  </r>
+  <r>
+    <n v="25230"/>
+    <x v="1"/>
+    <n v="185"/>
+    <s v="2017-11"/>
+  </r>
+  <r>
+    <n v="25231"/>
+    <x v="2"/>
+    <n v="160"/>
+    <s v="2017-11"/>
+  </r>
+  <r>
+    <n v="25232"/>
+    <x v="3"/>
+    <n v="393"/>
+    <s v="2017-11"/>
+  </r>
+  <r>
+    <n v="25233"/>
+    <x v="0"/>
+    <n v="114"/>
+    <s v="2017-12"/>
+  </r>
+  <r>
+    <n v="25234"/>
+    <x v="1"/>
+    <n v="156"/>
+    <s v="2017-12"/>
+  </r>
+  <r>
+    <n v="25235"/>
+    <x v="2"/>
+    <n v="132"/>
+    <s v="2017-12"/>
+  </r>
+  <r>
+    <n v="25236"/>
+    <x v="3"/>
+    <n v="385"/>
+    <s v="2017-12"/>
+  </r>
+  <r>
+    <n v="25237"/>
+    <x v="0"/>
+    <n v="128"/>
+    <s v="2018-01"/>
+  </r>
+  <r>
+    <n v="25238"/>
+    <x v="1"/>
+    <n v="156"/>
+    <s v="2018-01"/>
+  </r>
+  <r>
+    <n v="25239"/>
+    <x v="2"/>
+    <n v="156"/>
+    <s v="2018-01"/>
+  </r>
+  <r>
+    <n v="25240"/>
+    <x v="3"/>
+    <n v="375"/>
+    <s v="2018-01"/>
+  </r>
+  <r>
+    <n v="25241"/>
+    <x v="0"/>
+    <n v="145"/>
+    <s v="2018-02"/>
+  </r>
+  <r>
+    <n v="25242"/>
+    <x v="1"/>
+    <n v="182"/>
+    <s v="2018-02"/>
+  </r>
+  <r>
+    <n v="25243"/>
+    <x v="2"/>
+    <n v="149"/>
+    <s v="2018-02"/>
+  </r>
+  <r>
+    <n v="25244"/>
+    <x v="3"/>
+    <n v="344"/>
+    <s v="2018-02"/>
+  </r>
+  <r>
+    <n v="25245"/>
+    <x v="0"/>
+    <n v="177"/>
+    <s v="2018-03"/>
+  </r>
+  <r>
+    <n v="25246"/>
+    <x v="1"/>
+    <n v="235"/>
+    <s v="2018-03"/>
+  </r>
+  <r>
+    <n v="25247"/>
+    <x v="2"/>
+    <n v="187"/>
+    <s v="2018-03"/>
+  </r>
+  <r>
+    <n v="25248"/>
+    <x v="3"/>
+    <n v="538"/>
+    <s v="2018-03"/>
+  </r>
+  <r>
+    <n v="25249"/>
+    <x v="0"/>
+    <n v="188"/>
+    <s v="2018-04"/>
+  </r>
+  <r>
+    <n v="25250"/>
+    <x v="1"/>
+    <n v="238"/>
+    <s v="2018-04"/>
+  </r>
+  <r>
+    <n v="25251"/>
+    <x v="2"/>
+    <n v="239"/>
+    <s v="2018-04"/>
+  </r>
+  <r>
+    <n v="25252"/>
+    <x v="3"/>
+    <n v="657"/>
+    <s v="2018-04"/>
+  </r>
+  <r>
+    <n v="25253"/>
+    <x v="0"/>
+    <n v="229"/>
+    <s v="2018-05"/>
+  </r>
+  <r>
+    <n v="25254"/>
+    <x v="1"/>
+    <n v="337"/>
+    <s v="2018-05"/>
+  </r>
+  <r>
+    <n v="25255"/>
+    <x v="2"/>
+    <n v="302"/>
+    <s v="2018-05"/>
+  </r>
+  <r>
+    <n v="25256"/>
+    <x v="3"/>
+    <n v="880"/>
+    <s v="2018-05"/>
+  </r>
+  <r>
+    <n v="25257"/>
+    <x v="0"/>
+    <n v="279"/>
+    <s v="2018-06"/>
+  </r>
+  <r>
+    <n v="25258"/>
+    <x v="1"/>
+    <n v="337"/>
+    <s v="2018-06"/>
+  </r>
+  <r>
+    <n v="25259"/>
+    <x v="2"/>
+    <n v="338"/>
+    <s v="2018-06"/>
+  </r>
+  <r>
+    <n v="25260"/>
+    <x v="3"/>
+    <n v="964"/>
+    <s v="2018-06"/>
+  </r>
+  <r>
+    <n v="25261"/>
+    <x v="0"/>
+    <n v="324"/>
+    <s v="2018-07"/>
+  </r>
+  <r>
+    <n v="25262"/>
+    <x v="1"/>
+    <n v="408"/>
+    <s v="2018-07"/>
+  </r>
+  <r>
+    <n v="25263"/>
+    <x v="2"/>
+    <n v="347"/>
+    <s v="2018-07"/>
+  </r>
+  <r>
+    <n v="25264"/>
+    <x v="3"/>
+    <n v="1090"/>
+    <s v="2018-07"/>
+  </r>
+  <r>
+    <n v="25265"/>
+    <x v="0"/>
+    <n v="365"/>
+    <s v="2018-08"/>
+  </r>
+  <r>
+    <n v="25266"/>
+    <x v="1"/>
+    <n v="323"/>
+    <s v="2018-08"/>
+  </r>
+  <r>
+    <n v="25267"/>
+    <x v="2"/>
+    <n v="392"/>
+    <s v="2018-08"/>
+  </r>
+  <r>
+    <n v="25268"/>
+    <x v="3"/>
+    <n v="1117"/>
+    <s v="2018-08"/>
+  </r>
+  <r>
+    <n v="25269"/>
+    <x v="0"/>
+    <n v="209"/>
+    <s v="2018-09"/>
+  </r>
+  <r>
+    <n v="25270"/>
+    <x v="1"/>
+    <n v="256"/>
+    <s v="2018-09"/>
+  </r>
+  <r>
+    <n v="25271"/>
+    <x v="2"/>
+    <n v="216"/>
+    <s v="2018-09"/>
+  </r>
+  <r>
+    <n v="25272"/>
+    <x v="3"/>
+    <n v="719"/>
+    <s v="2018-09"/>
+  </r>
+  <r>
+    <n v="25273"/>
+    <x v="0"/>
+    <n v="187"/>
+    <s v="2018-10"/>
+  </r>
+  <r>
+    <n v="25274"/>
+    <x v="1"/>
+    <n v="227"/>
+    <s v="2018-10"/>
+  </r>
+  <r>
+    <n v="25275"/>
+    <x v="2"/>
+    <n v="186"/>
+    <s v="2018-10"/>
+  </r>
+  <r>
+    <n v="25276"/>
+    <x v="3"/>
+    <n v="582"/>
+    <s v="2018-10"/>
+  </r>
+  <r>
+    <n v="25277"/>
+    <x v="0"/>
+    <n v="140"/>
+    <s v="2018-11"/>
+  </r>
+  <r>
+    <n v="25278"/>
+    <x v="1"/>
+    <n v="199"/>
+    <s v="2018-11"/>
+  </r>
+  <r>
+    <n v="25279"/>
+    <x v="2"/>
+    <n v="169"/>
+    <s v="2018-11"/>
+  </r>
+  <r>
+    <n v="25280"/>
+    <x v="3"/>
+    <n v="397"/>
+    <s v="2018-11"/>
+  </r>
+  <r>
+    <n v="25281"/>
+    <x v="0"/>
+    <n v="108"/>
+    <s v="2018-12"/>
+  </r>
+  <r>
+    <n v="25282"/>
+    <x v="1"/>
+    <n v="157"/>
+    <s v="2018-12"/>
+  </r>
+  <r>
+    <n v="25283"/>
+    <x v="2"/>
+    <n v="123"/>
+    <s v="2018-12"/>
+  </r>
+  <r>
+    <n v="25284"/>
+    <x v="3"/>
+    <n v="329"/>
+    <s v="2018-12"/>
+  </r>
+  <r>
+    <n v="25285"/>
+    <x v="0"/>
+    <n v="123"/>
+    <s v="2019-01"/>
+  </r>
+  <r>
+    <n v="25286"/>
+    <x v="1"/>
+    <n v="162"/>
+    <s v="2019-01"/>
+  </r>
+  <r>
+    <n v="25287"/>
+    <x v="2"/>
+    <n v="151"/>
+    <s v="2019-01"/>
+  </r>
+  <r>
+    <n v="25288"/>
+    <x v="3"/>
+    <n v="341"/>
+    <s v="2019-01"/>
+  </r>
+  <r>
+    <n v="25289"/>
+    <x v="0"/>
+    <n v="143"/>
+    <s v="2019-02"/>
+  </r>
+  <r>
+    <n v="25290"/>
+    <x v="1"/>
+    <n v="190"/>
+    <s v="2019-02"/>
+  </r>
+  <r>
+    <n v="25291"/>
+    <x v="2"/>
+    <n v="158"/>
+    <s v="2019-02"/>
+  </r>
+  <r>
+    <n v="25292"/>
+    <x v="3"/>
+    <n v="382"/>
+    <s v="2019-02"/>
+  </r>
+  <r>
+    <n v="25293"/>
+    <x v="0"/>
+    <n v="170"/>
+    <s v="2019-03"/>
+  </r>
+  <r>
+    <n v="25294"/>
+    <x v="1"/>
+    <n v="236"/>
+    <s v="2019-03"/>
+  </r>
+  <r>
+    <n v="25295"/>
+    <x v="2"/>
+    <n v="240"/>
+    <s v="2019-03"/>
+  </r>
+  <r>
+    <n v="25296"/>
+    <x v="3"/>
+    <n v="576"/>
+    <s v="2019-03"/>
+  </r>
+  <r>
+    <n v="25297"/>
+    <x v="0"/>
+    <n v="193"/>
+    <s v="2019-04"/>
+  </r>
+  <r>
+    <n v="25298"/>
+    <x v="1"/>
+    <n v="290"/>
+    <s v="2019-04"/>
+  </r>
+  <r>
+    <n v="25299"/>
+    <x v="2"/>
+    <n v="237"/>
+    <s v="2019-04"/>
+  </r>
+  <r>
+    <n v="25300"/>
+    <x v="3"/>
+    <n v="724"/>
+    <s v="2019-04"/>
+  </r>
+  <r>
+    <n v="25301"/>
+    <x v="0"/>
+    <n v="235"/>
+    <s v="2019-05"/>
+  </r>
+  <r>
+    <n v="25302"/>
+    <x v="1"/>
+    <n v="336"/>
+    <s v="2019-05"/>
+  </r>
+  <r>
+    <n v="25303"/>
+    <x v="2"/>
+    <n v="285"/>
+    <s v="2019-05"/>
+  </r>
+  <r>
+    <n v="25304"/>
+    <x v="3"/>
+    <n v="879"/>
+    <s v="2019-05"/>
+  </r>
+  <r>
+    <n v="25305"/>
+    <x v="0"/>
+    <n v="242"/>
+    <s v="2019-06"/>
+  </r>
+  <r>
+    <n v="25306"/>
+    <x v="1"/>
+    <n v="315"/>
+    <s v="2019-06"/>
+  </r>
+  <r>
+    <n v="25307"/>
+    <x v="2"/>
+    <n v="280"/>
+    <s v="2019-06"/>
+  </r>
+  <r>
+    <n v="25308"/>
+    <x v="3"/>
+    <n v="901"/>
+    <s v="2019-06"/>
+  </r>
+  <r>
+    <n v="25309"/>
+    <x v="0"/>
+    <n v="308"/>
+    <s v="2019-07"/>
+  </r>
+  <r>
+    <n v="25310"/>
+    <x v="1"/>
+    <n v="407"/>
+    <s v="2019-07"/>
+  </r>
+  <r>
+    <n v="25311"/>
+    <x v="2"/>
+    <n v="323"/>
+    <s v="2019-07"/>
+  </r>
+  <r>
+    <n v="25312"/>
+    <x v="3"/>
+    <n v="1079"/>
+    <s v="2019-07"/>
+  </r>
+  <r>
+    <n v="25313"/>
+    <x v="0"/>
+    <n v="281"/>
+    <s v="2019-08"/>
+  </r>
+  <r>
+    <n v="25314"/>
+    <x v="1"/>
+    <n v="384"/>
+    <s v="2019-08"/>
+  </r>
+  <r>
+    <n v="25315"/>
+    <x v="2"/>
+    <n v="329"/>
+    <s v="2019-08"/>
+  </r>
+  <r>
+    <n v="25316"/>
+    <x v="3"/>
+    <n v="1011"/>
+    <s v="2019-08"/>
+  </r>
+  <r>
+    <n v="25317"/>
+    <x v="0"/>
+    <n v="220"/>
+    <s v="2019-09"/>
+  </r>
+  <r>
+    <n v="25318"/>
+    <x v="1"/>
+    <n v="247"/>
+    <s v="2019-09"/>
+  </r>
+  <r>
+    <n v="25319"/>
+    <x v="2"/>
+    <n v="221"/>
+    <s v="2019-09"/>
+  </r>
+  <r>
+    <n v="25320"/>
+    <x v="3"/>
+    <n v="738"/>
+    <s v="2019-09"/>
+  </r>
+  <r>
+    <n v="25321"/>
+    <x v="0"/>
+    <n v="150"/>
+    <s v="2019-10"/>
+  </r>
+  <r>
+    <n v="25322"/>
+    <x v="1"/>
+    <n v="228"/>
+    <s v="2019-10"/>
+  </r>
+  <r>
+    <n v="25323"/>
+    <x v="2"/>
+    <n v="172"/>
+    <s v="2019-10"/>
+  </r>
+  <r>
+    <n v="25324"/>
+    <x v="3"/>
+    <n v="576"/>
+    <s v="2019-10"/>
+  </r>
+  <r>
+    <n v="25325"/>
+    <x v="0"/>
+    <n v="120"/>
+    <s v="2019-11"/>
+  </r>
+  <r>
+    <n v="25326"/>
+    <x v="1"/>
+    <n v="198"/>
+    <s v="2019-11"/>
+  </r>
+  <r>
+    <n v="25327"/>
+    <x v="2"/>
+    <n v="156"/>
+    <s v="2019-11"/>
+  </r>
+  <r>
+    <n v="25328"/>
+    <x v="3"/>
+    <n v="433"/>
+    <s v="2019-11"/>
+  </r>
+  <r>
+    <n v="25329"/>
+    <x v="0"/>
+    <n v="122"/>
+    <s v="2019-12"/>
+  </r>
+  <r>
+    <n v="25330"/>
+    <x v="1"/>
+    <n v="187"/>
+    <s v="2019-12"/>
+  </r>
+  <r>
+    <n v="25331"/>
+    <x v="2"/>
+    <n v="153"/>
+    <s v="2019-12"/>
+  </r>
+  <r>
+    <n v="25332"/>
+    <x v="3"/>
+    <n v="393"/>
+    <s v="2019-12"/>
+  </r>
+  <r>
+    <n v="25333"/>
+    <x v="0"/>
+    <n v="130"/>
+    <s v="2020-01"/>
+  </r>
+  <r>
+    <n v="25334"/>
+    <x v="1"/>
+    <n v="168"/>
+    <s v="2020-01"/>
+  </r>
+  <r>
+    <n v="25335"/>
+    <x v="2"/>
+    <n v="171"/>
+    <s v="2020-01"/>
+  </r>
+  <r>
+    <n v="25336"/>
+    <x v="3"/>
+    <n v="426"/>
+    <s v="2020-01"/>
+  </r>
+  <r>
+    <n v="25337"/>
+    <x v="0"/>
+    <n v="130"/>
+    <s v="2020-02"/>
+  </r>
+  <r>
+    <n v="25338"/>
+    <x v="1"/>
+    <n v="184"/>
+    <s v="2020-02"/>
+  </r>
+  <r>
+    <n v="25339"/>
+    <x v="2"/>
+    <n v="160"/>
+    <s v="2020-02"/>
+  </r>
+  <r>
+    <n v="25340"/>
+    <x v="3"/>
+    <n v="434"/>
+    <s v="2020-02"/>
+  </r>
+  <r>
+    <n v="25341"/>
+    <x v="0"/>
+    <n v="101"/>
+    <s v="2020-03"/>
+  </r>
+  <r>
+    <n v="25342"/>
+    <x v="1"/>
+    <n v="122"/>
+    <s v="2020-03"/>
+  </r>
+  <r>
+    <n v="25343"/>
+    <x v="2"/>
+    <n v="99"/>
+    <s v="2020-03"/>
+  </r>
+  <r>
+    <n v="25344"/>
+    <x v="3"/>
+    <n v="294"/>
+    <s v="2020-03"/>
+  </r>
+  <r>
+    <n v="25345"/>
+    <x v="3"/>
+    <n v="47"/>
+    <s v="2020-04"/>
+  </r>
+  <r>
+    <n v="25346"/>
+    <x v="3"/>
+    <n v="123"/>
+    <s v="2020-05"/>
+  </r>
+  <r>
+    <n v="25347"/>
+    <x v="1"/>
+    <n v="167"/>
+    <s v="2020-06"/>
+  </r>
+  <r>
+    <n v="25348"/>
+    <x v="2"/>
+    <n v="222"/>
+    <s v="2020-06"/>
+  </r>
+  <r>
+    <n v="25349"/>
+    <x v="3"/>
+    <n v="248"/>
+    <s v="2020-06"/>
+  </r>
+  <r>
+    <n v="25350"/>
+    <x v="1"/>
+    <n v="718"/>
+    <s v="2020-07"/>
+  </r>
+  <r>
+    <n v="25351"/>
+    <x v="2"/>
+    <n v="782"/>
+    <s v="2020-07"/>
+  </r>
+  <r>
+    <n v="25352"/>
+    <x v="1"/>
+    <n v="776"/>
+    <s v="2020-08"/>
+  </r>
+  <r>
+    <n v="25353"/>
+    <x v="2"/>
+    <n v="637"/>
+    <s v="2020-08"/>
+  </r>
+  <r>
+    <n v="25354"/>
+    <x v="1"/>
+    <n v="864"/>
+    <s v="2020-09"/>
+  </r>
+  <r>
+    <n v="25355"/>
+    <x v="2"/>
+    <n v="569"/>
+    <s v="2020-09"/>
+  </r>
+  <r>
+    <n v="25356"/>
+    <x v="1"/>
+    <n v="536"/>
+    <s v="2020-10"/>
+  </r>
+  <r>
+    <n v="25357"/>
+    <x v="2"/>
+    <n v="581"/>
+    <s v="2020-10"/>
+  </r>
+  <r>
+    <n v="25358"/>
+    <x v="1"/>
+    <n v="366"/>
+    <s v="2020-11"/>
+  </r>
+  <r>
+    <n v="25359"/>
+    <x v="2"/>
+    <n v="320"/>
+    <s v="2020-11"/>
+  </r>
+  <r>
+    <n v="25360"/>
+    <x v="1"/>
+    <n v="168"/>
+    <s v="2020-12"/>
+  </r>
+  <r>
+    <n v="25361"/>
+    <x v="2"/>
+    <n v="200"/>
+    <s v="2020-12"/>
+  </r>
+  <r>
+    <n v="25362"/>
+    <x v="1"/>
+    <n v="286"/>
+    <s v="2021-01"/>
+  </r>
+  <r>
+    <n v="25363"/>
+    <x v="2"/>
+    <n v="78"/>
+    <s v="2021-01"/>
+  </r>
+  <r>
+    <n v="25364"/>
+    <x v="1"/>
+    <n v="427"/>
+    <s v="2021-02"/>
+  </r>
+  <r>
+    <n v="25365"/>
+    <x v="2"/>
+    <n v="108"/>
+    <s v="2021-02"/>
+  </r>
+  <r>
+    <n v="25366"/>
+    <x v="1"/>
+    <n v="631"/>
+    <s v="2021-03"/>
+  </r>
+  <r>
+    <n v="25367"/>
+    <x v="2"/>
+    <n v="285"/>
+    <s v="2021-03"/>
+  </r>
+  <r>
+    <n v="25368"/>
+    <x v="0"/>
+    <n v="1"/>
+    <s v="2021-04"/>
+  </r>
+  <r>
+    <n v="25369"/>
+    <x v="1"/>
+    <n v="560"/>
+    <s v="2021-04"/>
+  </r>
+  <r>
+    <n v="25370"/>
+    <x v="2"/>
+    <n v="191"/>
+    <s v="2021-04"/>
+  </r>
+  <r>
+    <n v="25371"/>
+    <x v="1"/>
+    <n v="518"/>
+    <s v="2021-05"/>
+  </r>
+  <r>
+    <n v="25372"/>
+    <x v="2"/>
+    <n v="187"/>
+    <s v="2021-05"/>
+  </r>
+  <r>
+    <n v="25373"/>
+    <x v="1"/>
+    <n v="677"/>
+    <s v="2021-06"/>
+  </r>
+  <r>
+    <n v="25374"/>
+    <x v="2"/>
+    <n v="215"/>
+    <s v="2021-06"/>
+  </r>
+  <r>
+    <n v="25375"/>
+    <x v="3"/>
+    <n v="3"/>
+    <s v="2021-06"/>
+  </r>
+  <r>
+    <n v="25376"/>
+    <x v="1"/>
+    <n v="997"/>
+    <s v="2021-07"/>
+  </r>
+  <r>
+    <n v="25377"/>
+    <x v="2"/>
+    <n v="375"/>
+    <s v="2021-07"/>
+  </r>
+  <r>
+    <n v="25378"/>
+    <x v="1"/>
+    <n v="372"/>
+    <s v="2021-08"/>
+  </r>
+  <r>
+    <n v="25379"/>
+    <x v="2"/>
+    <n v="266"/>
+    <s v="2021-08"/>
+  </r>
+  <r>
+    <n v="25380"/>
+    <x v="3"/>
+    <n v="922"/>
+    <s v="2021-08"/>
+  </r>
+  <r>
+    <n v="25381"/>
+    <x v="3"/>
+    <n v="1773"/>
+    <s v="2021-09"/>
+  </r>
+  <r>
+    <n v="25382"/>
+    <x v="3"/>
+    <n v="1413"/>
+    <s v="2021-10"/>
+  </r>
+  <r>
+    <n v="25383"/>
+    <x v="3"/>
+    <n v="783"/>
+    <s v="2021-11"/>
+  </r>
+  <r>
+    <n v="25384"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="2021-12"/>
+  </r>
+  <r>
+    <n v="25385"/>
+    <x v="3"/>
+    <n v="689"/>
+    <s v="2021-12"/>
+  </r>
+  <r>
+    <n v="25386"/>
+    <x v="3"/>
+    <n v="472"/>
+    <s v="2022-01"/>
+  </r>
+  <r>
+    <n v="25387"/>
+    <x v="3"/>
+    <n v="536"/>
+    <s v="2022-02"/>
+  </r>
+  <r>
+    <n v="25388"/>
+    <x v="3"/>
+    <n v="1220"/>
+    <s v="2022-03"/>
+  </r>
+  <r>
+    <n v="25389"/>
+    <x v="3"/>
+    <n v="1265"/>
+    <s v="2022-04"/>
+  </r>
+  <r>
+    <n v="25390"/>
+    <x v="3"/>
+    <n v="1269"/>
+    <s v="2022-05"/>
+  </r>
+  <r>
+    <n v="25391"/>
+    <x v="1"/>
+    <n v="455"/>
+    <s v="2022-06"/>
+  </r>
+  <r>
+    <n v="25392"/>
+    <x v="3"/>
+    <n v="1658"/>
+    <s v="2022-06"/>
+  </r>
+  <r>
+    <n v="25393"/>
+    <x v="1"/>
+    <n v="559"/>
+    <s v="2022-07"/>
+  </r>
+  <r>
+    <n v="25394"/>
+    <x v="3"/>
+    <n v="1507"/>
+    <s v="2022-07"/>
+  </r>
+  <r>
+    <n v="25395"/>
+    <x v="1"/>
+    <n v="647"/>
+    <s v="2022-08"/>
+  </r>
+  <r>
+    <n v="25396"/>
+    <x v="3"/>
+    <n v="1656"/>
+    <s v="2022-08"/>
+  </r>
+  <r>
+    <n v="25397"/>
+    <x v="1"/>
+    <n v="467"/>
+    <s v="2022-09"/>
+  </r>
+  <r>
+    <n v="25398"/>
+    <x v="3"/>
+    <n v="1108"/>
+    <s v="2022-09"/>
+  </r>
+  <r>
+    <n v="25399"/>
+    <x v="1"/>
+    <n v="304"/>
+    <s v="2022-10"/>
+  </r>
+  <r>
+    <n v="25400"/>
+    <x v="3"/>
+    <n v="611"/>
+    <s v="2022-10"/>
+  </r>
+  <r>
+    <n v="25401"/>
+    <x v="1"/>
+    <n v="329"/>
+    <s v="2022-11"/>
+  </r>
+  <r>
+    <n v="25402"/>
+    <x v="3"/>
+    <n v="476"/>
+    <s v="2022-11"/>
+  </r>
+  <r>
+    <n v="25403"/>
+    <x v="1"/>
+    <n v="128"/>
+    <s v="2022-12"/>
+  </r>
+  <r>
+    <n v="25404"/>
+    <x v="3"/>
+    <n v="556"/>
+    <s v="2022-12"/>
+  </r>
+  <r>
+    <n v="25405"/>
+    <x v="1"/>
+    <n v="149"/>
+    <s v="2023-01"/>
+  </r>
+  <r>
+    <n v="25406"/>
+    <x v="3"/>
+    <n v="563"/>
+    <s v="2023-01"/>
+  </r>
+  <r>
+    <n v="25407"/>
+    <x v="1"/>
+    <n v="156"/>
+    <s v="2023-02"/>
+  </r>
+  <r>
+    <n v="25408"/>
+    <x v="3"/>
+    <n v="617"/>
+    <s v="2023-02"/>
+  </r>
+  <r>
+    <n v="25409"/>
+    <x v="1"/>
+    <n v="215"/>
+    <s v="2023-03"/>
+  </r>
+  <r>
+    <n v="25410"/>
+    <x v="3"/>
+    <n v="929"/>
+    <s v="2023-03"/>
+  </r>
+  <r>
+    <n v="25411"/>
+    <x v="1"/>
+    <n v="318"/>
+    <s v="2023-04"/>
+  </r>
+  <r>
+    <n v="25412"/>
+    <x v="3"/>
+    <n v="1086"/>
+    <s v="2023-04"/>
+  </r>
+  <r>
+    <n v="25413"/>
+    <x v="1"/>
+    <n v="305"/>
+    <s v="2023-05"/>
+  </r>
+  <r>
+    <n v="25414"/>
+    <x v="3"/>
+    <n v="1507"/>
+    <s v="2023-05"/>
+  </r>
+  <r>
+    <n v="25415"/>
+    <x v="1"/>
+    <n v="416"/>
+    <s v="2023-06"/>
+  </r>
+  <r>
+    <n v="25416"/>
+    <x v="3"/>
+    <n v="1507"/>
+    <s v="2023-06"/>
+  </r>
+  <r>
+    <n v="25417"/>
+    <x v="1"/>
+    <n v="439"/>
+    <s v="2023-07"/>
+  </r>
+  <r>
+    <n v="25418"/>
+    <x v="3"/>
+    <n v="1628"/>
+    <s v="2023-07"/>
+  </r>
+  <r>
+    <n v="25419"/>
+    <x v="1"/>
+    <n v="412"/>
+    <s v="2023-08"/>
+  </r>
+  <r>
+    <n v="25420"/>
+    <x v="3"/>
+    <n v="1649"/>
+    <s v="2023-08"/>
+  </r>
+  <r>
+    <n v="25421"/>
+    <x v="1"/>
+    <n v="266"/>
+    <s v="2023-09"/>
+  </r>
+  <r>
+    <n v="25422"/>
+    <x v="3"/>
+    <n v="1156"/>
+    <s v="2023-09"/>
+  </r>
+  <r>
+    <n v="25423"/>
+    <x v="1"/>
+    <n v="296"/>
+    <s v="2023-10"/>
+  </r>
+  <r>
+    <n v="25424"/>
+    <x v="3"/>
+    <n v="811"/>
+    <s v="2023-10"/>
+  </r>
+  <r>
+    <n v="25425"/>
+    <x v="1"/>
+    <n v="260"/>
+    <s v="2023-11"/>
+  </r>
+  <r>
+    <n v="25426"/>
+    <x v="3"/>
+    <n v="606"/>
+    <s v="2023-11"/>
+  </r>
+  <r>
+    <n v="25427"/>
+    <x v="1"/>
+    <n v="99"/>
+    <s v="2023-12"/>
+  </r>
+  <r>
+    <n v="25428"/>
+    <x v="3"/>
+    <n v="646"/>
+    <s v="2023-12"/>
+  </r>
+  <r>
+    <n v="25429"/>
+    <x v="1"/>
+    <n v="135"/>
+    <s v="2024-01"/>
+  </r>
+  <r>
+    <n v="25430"/>
+    <x v="3"/>
+    <n v="840"/>
+    <s v="2024-01"/>
+  </r>
+  <r>
+    <n v="25431"/>
+    <x v="1"/>
+    <n v="193"/>
+    <s v="2024-02"/>
+  </r>
+  <r>
+    <n v="25432"/>
+    <x v="3"/>
+    <n v="800"/>
+    <s v="2024-02"/>
+  </r>
+  <r>
+    <n v="25433"/>
+    <x v="1"/>
+    <n v="114"/>
+    <s v="2024-03"/>
+  </r>
+  <r>
+    <n v="25434"/>
+    <x v="3"/>
+    <n v="1116"/>
+    <s v="2024-03"/>
+  </r>
+  <r>
+    <n v="25435"/>
+    <x v="1"/>
+    <n v="270"/>
+    <s v="2024-04"/>
+  </r>
+  <r>
+    <n v="25436"/>
+    <x v="3"/>
+    <n v="1279"/>
+    <s v="2024-04"/>
+  </r>
+  <r>
+    <n v="25437"/>
+    <x v="1"/>
+    <n v="409"/>
+    <s v="2024-05"/>
+  </r>
+  <r>
+    <n v="25438"/>
+    <x v="3"/>
+    <n v="1347"/>
+    <s v="2024-05"/>
+  </r>
+  <r>
+    <n v="25439"/>
+    <x v="1"/>
+    <n v="394"/>
+    <s v="2024-06"/>
+  </r>
+  <r>
+    <n v="25440"/>
+    <x v="3"/>
+    <n v="1355"/>
+    <s v="2024-06"/>
+  </r>
+  <r>
+    <n v="25441"/>
+    <x v="1"/>
+    <n v="670"/>
+    <s v="2024-07"/>
+  </r>
+  <r>
+    <n v="25442"/>
+    <x v="3"/>
+    <n v="1545"/>
+    <s v="2024-07"/>
+  </r>
+  <r>
+    <n v="25443"/>
+    <x v="1"/>
+    <n v="675"/>
+    <s v="2024-08"/>
+  </r>
+  <r>
+    <n v="25444"/>
+    <x v="3"/>
+    <n v="1406"/>
+    <s v="2024-08"/>
+  </r>
+  <r>
+    <n v="25445"/>
+    <x v="1"/>
+    <n v="433"/>
+    <s v="2024-09"/>
+  </r>
+  <r>
+    <n v="25446"/>
+    <x v="3"/>
+    <n v="944"/>
+    <s v="2024-09"/>
+  </r>
+  <r>
+    <n v="25447"/>
+    <x v="1"/>
+    <n v="434"/>
+    <s v="2024-10"/>
+  </r>
+  <r>
+    <n v="25448"/>
+    <x v="3"/>
+    <n v="772"/>
+    <s v="2024-10"/>
+  </r>
+  <r>
+    <n v="25449"/>
+    <x v="1"/>
+    <n v="321"/>
+    <s v="2024-11"/>
+  </r>
+  <r>
+    <n v="25450"/>
+    <x v="3"/>
+    <n v="556"/>
+    <s v="2024-11"/>
+  </r>
+  <r>
+    <n v="25451"/>
+    <x v="1"/>
+    <n v="254"/>
+    <s v="2024-12"/>
+  </r>
+  <r>
+    <n v="25452"/>
+    <x v="3"/>
+    <n v="529"/>
+    <s v="2024-12"/>
+  </r>
+  <r>
+    <n v="25453"/>
+    <x v="1"/>
+    <n v="309"/>
+    <s v="2025-01"/>
+  </r>
+  <r>
+    <n v="25454"/>
+    <x v="3"/>
+    <n v="784"/>
+    <s v="2025-01"/>
+  </r>
+  <r>
+    <n v="25455"/>
+    <x v="1"/>
+    <n v="262"/>
+    <s v="2025-02"/>
+  </r>
+  <r>
+    <n v="25456"/>
+    <x v="3"/>
+    <n v="671"/>
+    <s v="2025-02"/>
+  </r>
+  <r>
+    <n v="25457"/>
+    <x v="1"/>
+    <n v="297"/>
+    <s v="2025-03"/>
+  </r>
+  <r>
+    <n v="25458"/>
+    <x v="3"/>
+    <n v="801"/>
+    <s v="2025-03"/>
+  </r>
+  <r>
+    <n v="25459"/>
+    <x v="1"/>
+    <n v="365"/>
+    <s v="2025-04"/>
+  </r>
+  <r>
+    <n v="25460"/>
+    <x v="3"/>
+    <n v="935"/>
+    <s v="2025-04"/>
+  </r>
+  <r>
+    <n v="25461"/>
+    <x v="1"/>
+    <n v="607"/>
+    <s v="2025-05"/>
+  </r>
+  <r>
+    <n v="25462"/>
+    <x v="3"/>
+    <n v="1132"/>
+    <s v="2025-05"/>
+  </r>
+  <r>
+    <n v="25463"/>
+    <x v="1"/>
+    <n v="568"/>
+    <s v="2025-06"/>
+  </r>
+  <r>
+    <n v="25464"/>
+    <x v="3"/>
+    <n v="1546"/>
+    <s v="2025-06"/>
+  </r>
+  <r>
+    <n v="25465"/>
+    <x v="1"/>
+    <n v="611"/>
+    <s v="2025-07"/>
+  </r>
+  <r>
+    <n v="25466"/>
+    <x v="3"/>
+    <n v="1706"/>
+    <s v="2025-07"/>
+  </r>
+  <r>
+    <n v="25467"/>
+    <x v="1"/>
+    <n v="549"/>
+    <s v="2025-08"/>
+  </r>
+  <r>
+    <n v="25468"/>
+    <x v="3"/>
+    <n v="1410"/>
+    <s v="2025-08"/>
+  </r>
+  <r>
+    <n v="25469"/>
+    <x v="1"/>
+    <n v="387"/>
+    <s v="2025-09"/>
+  </r>
+  <r>
+    <n v="25470"/>
+    <x v="3"/>
+    <n v="1101"/>
+    <s v="2025-09"/>
+  </r>
+  <r>
+    <n v="25471"/>
+    <x v="1"/>
+    <n v="241"/>
+    <s v="2025-10"/>
+  </r>
+  <r>
+    <n v="25472"/>
+    <x v="3"/>
+    <n v="878"/>
+    <s v="2025-10"/>
+  </r>
+  <r>
+    <n v="25473"/>
+    <x v="1"/>
+    <n v="118"/>
+    <s v="2025-11"/>
+  </r>
+  <r>
+    <n v="25474"/>
+    <x v="3"/>
+    <n v="700"/>
+    <s v="2025-11"/>
+  </r>
+  <r>
+    <n v="25475"/>
+    <x v="1"/>
+    <n v="249"/>
+    <s v="2025-12"/>
+  </r>
+  <r>
+    <n v="25476"/>
+    <x v="3"/>
+    <n v="539"/>
+    <s v="2025-12"/>
+  </r>
+  <r>
+    <n v="25477"/>
+    <x v="1"/>
+    <n v="270"/>
+    <s v="2026-01"/>
+  </r>
+  <r>
+    <n v="25478"/>
+    <x v="3"/>
+    <n v="575"/>
+    <s v="2026-01"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of MARRIAGE_LICENSES" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1427,10 +6173,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>19624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>50960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>30512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>126182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="3">
+        <v>227278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>